<commit_message>
added figures and screenshots
</commit_message>
<xml_diff>
--- a/writing/master-thesis/figures/uncertainty_measures.xlsx
+++ b/writing/master-thesis/figures/uncertainty_measures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\OneDrive - mail.uni-paderborn.de\Studium\Master\4. Semester\Master thesis\repo\writing\master-thesis\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61047558-764D-46EC-8A44-FAF9F561F244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DE9F66-BCE4-407B-858E-83DF44F299E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{49D5EF2A-3B15-46FD-9012-024655AACA56}"/>
+    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{49D5EF2A-3B15-46FD-9012-024655AACA56}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="4" r:id="rId1"/>
@@ -5750,7 +5750,7 @@
   <dimension ref="G2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5767,8 +5767,9 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>0</v>
+      <c r="H3" t="e">
+        <f>-(G3*LOG(G3,2) + (1-G3) *LOG(1-G3,2))</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="4" spans="7:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated xlsx with uncertainty metrics
</commit_message>
<xml_diff>
--- a/writing/master-thesis/figures/uncertainty_measures.xlsx
+++ b/writing/master-thesis/figures/uncertainty_measures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\OneDrive - mail.uni-paderborn.de\Studium\Master\4. Semester\Master thesis\repo\writing\master-thesis\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunipaderbornde-my.sharepoint.com/personal/chschaef_mail_uni-paderborn_de/Documents/Studium/Master/4. Semester/Master thesis/repo/writing/master-thesis/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862339D8-50D4-4A9A-8B0E-6A89B63D3567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{862339D8-50D4-4A9A-8B0E-6A89B63D3567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{476E9451-C2CD-40E2-9F22-C993E88DA5C7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="829" activeTab="4" xr2:uid="{49D5EF2A-3B15-46FD-9012-024655AACA56}"/>
   </bookViews>
@@ -24820,7 +24820,7 @@
   <dimension ref="G2:H23"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25033,7 +25033,7 @@
   <dimension ref="B2:C23"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25060,7 +25060,7 @@
         <v>0.05</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C12" si="0">1-((1-B4)-B4)</f>
+        <f>1-(MAX(B4,1-B4)-MIN(B4,1-B4))</f>
         <v>0.10000000000000009</v>
       </c>
     </row>
@@ -25069,7 +25069,7 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C5:C23" si="0">1-(MAX(B5,1-B5)-MIN(B5,1-B5))</f>
         <v>0.19999999999999996</v>
       </c>
     </row>
@@ -25141,7 +25141,7 @@
         <v>0.5</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C22" si="1">1-(B13-(1-B13))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -25150,7 +25150,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
@@ -25159,7 +25159,7 @@
         <v>0.6</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
@@ -25168,7 +25168,7 @@
         <v>0.65</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
@@ -25177,7 +25177,7 @@
         <v>0.7</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -25186,7 +25186,7 @@
         <v>0.75</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -25195,7 +25195,7 @@
         <v>0.8</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.39999999999999991</v>
       </c>
     </row>
@@ -25204,7 +25204,7 @@
         <v>0.85</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -25213,7 +25213,7 @@
         <v>0.9</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.19999999999999996</v>
       </c>
     </row>
@@ -25222,7 +25222,7 @@
         <v>0.95</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.10000000000000009</v>
       </c>
     </row>
@@ -25231,7 +25231,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23" si="2">1-(B23-(1-B23))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -25246,7 +25246,7 @@
   <dimension ref="B2:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25264,7 +25264,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <f>B3/(1-B3)</f>
+        <f>MIN(B3,1-B3) / MAX(B3,1-B3)</f>
         <v>0</v>
       </c>
     </row>
@@ -25273,7 +25273,7 @@
         <v>0.05</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C13" si="0">B4/(1-B4)</f>
+        <f>MIN(B4,1-B4) / MAX(B4,1-B4)</f>
         <v>5.2631578947368425E-2</v>
       </c>
     </row>
@@ -25282,7 +25282,7 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C5:C23" si="0">MIN(B5,1-B5) / MAX(B5,1-B5)</f>
         <v>0.11111111111111112</v>
       </c>
     </row>
@@ -25363,7 +25363,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C22" si="1">(1-B14)/B14</f>
+        <f t="shared" si="0"/>
         <v>0.81818181818181801</v>
       </c>
     </row>
@@ -25372,7 +25372,7 @@
         <v>0.6</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.66666666666666674</v>
       </c>
     </row>
@@ -25381,7 +25381,7 @@
         <v>0.65</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.53846153846153844</v>
       </c>
     </row>
@@ -25390,7 +25390,7 @@
         <v>0.7</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.42857142857142866</v>
       </c>
     </row>
@@ -25399,7 +25399,7 @@
         <v>0.75</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -25408,7 +25408,7 @@
         <v>0.8</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.24999999999999994</v>
       </c>
     </row>
@@ -25417,7 +25417,7 @@
         <v>0.85</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.17647058823529416</v>
       </c>
     </row>
@@ -25426,7 +25426,7 @@
         <v>0.9</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.11111111111111108</v>
       </c>
     </row>
@@ -25435,7 +25435,7 @@
         <v>0.95</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.2631578947368474E-2</v>
       </c>
     </row>
@@ -25444,7 +25444,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23" si="2">(1-B23)/B23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edited Introduction + Negative Sampling, evaluation figures 5k epochs
</commit_message>
<xml_diff>
--- a/writing/master-thesis/figures/uncertainty_measures.xlsx
+++ b/writing/master-thesis/figures/uncertainty_measures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunipaderbornde-my.sharepoint.com/personal/chschaef_mail_uni-paderborn_de/Documents/Studium/Master/4. Semester/Master thesis/repo/writing/master-thesis/figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\OneDrive - mail.uni-paderborn.de\Studium\Master\4. Semester\Master thesis\repo\writing\master-thesis\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{862339D8-50D4-4A9A-8B0E-6A89B63D3567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{476E9451-C2CD-40E2-9F22-C993E88DA5C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBEC120-83D3-465B-9917-203FA848605E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="829" activeTab="4" xr2:uid="{49D5EF2A-3B15-46FD-9012-024655AACA56}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="829" activeTab="2" xr2:uid="{49D5EF2A-3B15-46FD-9012-024655AACA56}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="4" r:id="rId1"/>
@@ -1298,7 +1298,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1316,6 +1316,7 @@
         <c:crossAx val="340273648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="340273648"/>
@@ -1424,7 +1425,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2047,7 +2048,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2173,7 +2174,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3355,7 +3356,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3481,7 +3482,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -23936,16 +23937,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>561973</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>61230</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>57147</xdr:rowOff>
+      <xdr:rowOff>122462</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>504716</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>55090</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>494225</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -24696,8 +24697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83B30F8-8253-4049-A309-D84692CF1DE7}">
   <dimension ref="G2:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24819,8 +24820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C8265D-8433-41D2-86BE-562B7E91A5E0}">
   <dimension ref="G2:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25245,7 +25246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B4B6D1-3188-48DA-9FCE-E1C39EE7601E}">
   <dimension ref="B2:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>

</xml_diff>